<commit_message>
Made following changes: - add progress bar for generating xml menu - add common method to show status (ie process records, success, fail etc) after generating xml - updated excel downloading from live site (update changes up to 9 Feb 2017) - after updating excel, changes mapping excel accordingly to include new changes
</commit_message>
<xml_diff>
--- a/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_PCMC/FF_Old_New_QuestionMapping_Parag.xlsx
+++ b/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_PCMC/FF_Old_New_QuestionMapping_Parag.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FFOldNewQuesMapping" sheetId="1" r:id="rId1"/>
     <sheet name="FFOldNewOptionMapping" sheetId="2" r:id="rId2"/>
     <sheet name="FFOptionMappingFinal" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="1320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="1338">
   <si>
     <t>begin_group</t>
   </si>
@@ -3768,9 +3768,6 @@
     <t>40</t>
   </si>
   <si>
-    <t>Rickshaw Puller</t>
-  </si>
-  <si>
     <t>41</t>
   </si>
   <si>
@@ -3846,9 +3843,6 @@
     <t>53</t>
   </si>
   <si>
-    <t>Aaya</t>
-  </si>
-  <si>
     <t>54</t>
   </si>
   <si>
@@ -4000,6 +3994,66 @@
   </si>
   <si>
     <t>07</t>
+  </si>
+  <si>
+    <t>6,30</t>
+  </si>
+  <si>
+    <t>8,64,74</t>
+  </si>
+  <si>
+    <t>9,10,88</t>
+  </si>
+  <si>
+    <t>11,60</t>
+  </si>
+  <si>
+    <t>16,32,36</t>
+  </si>
+  <si>
+    <t>20,21</t>
+  </si>
+  <si>
+    <t>45,47,56</t>
+  </si>
+  <si>
+    <t>46,48</t>
+  </si>
+  <si>
+    <t>67,68,78,86</t>
+  </si>
+  <si>
+    <t>55,63,75,98</t>
+  </si>
+  <si>
+    <t>54,80,99</t>
+  </si>
+  <si>
+    <t>Rickshaw/Puller/Driver</t>
+  </si>
+  <si>
+    <t>Auto Rickshaw/Cycle-Rickshaw driver</t>
+  </si>
+  <si>
+    <t>Hospital work</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>Compounder</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Salesman</t>
   </si>
 </sst>
 </file>
@@ -4420,7 +4474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5553,9 +5607,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M622"/>
+  <dimension ref="B1:M625"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
+      <selection activeCell="A602" sqref="A602:XFD604"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13202,8 +13258,8 @@
       <c r="I540" s="5">
         <v>434</v>
       </c>
-      <c r="J540">
-        <v>6</v>
+      <c r="J540" t="s">
+        <v>1318</v>
       </c>
       <c r="L540" s="5">
         <v>434</v>
@@ -13254,8 +13310,8 @@
       <c r="I542" s="5">
         <v>434</v>
       </c>
-      <c r="J542">
-        <v>8</v>
+      <c r="J542" t="s">
+        <v>1319</v>
       </c>
       <c r="L542" s="5">
         <v>434</v>
@@ -13282,7 +13338,7 @@
         <v>434</v>
       </c>
       <c r="J543" s="20" t="s">
-        <v>1180</v>
+        <v>1320</v>
       </c>
       <c r="L543" s="19">
         <v>434</v>
@@ -13307,8 +13363,8 @@
       <c r="I544" s="5">
         <v>434</v>
       </c>
-      <c r="J544">
-        <v>11</v>
+      <c r="J544" t="s">
+        <v>1321</v>
       </c>
       <c r="L544" s="5">
         <v>434</v>
@@ -13437,8 +13493,8 @@
       <c r="I549" s="5">
         <v>434</v>
       </c>
-      <c r="J549">
-        <v>16</v>
+      <c r="J549" t="s">
+        <v>1322</v>
       </c>
       <c r="L549" s="5">
         <v>434</v>
@@ -13542,6 +13598,9 @@
       <c r="I553" s="19">
         <v>434</v>
       </c>
+      <c r="J553" s="17" t="s">
+        <v>1323</v>
+      </c>
       <c r="L553" s="19">
         <v>434</v>
       </c>
@@ -14073,8 +14132,8 @@
       <c r="C574" s="16" t="s">
         <v>1241</v>
       </c>
-      <c r="D574" s="16" t="s">
-        <v>1242</v>
+      <c r="D574" s="1" t="s">
+        <v>1329</v>
       </c>
       <c r="G574" s="18"/>
       <c r="H574" s="17" t="s">
@@ -14083,8 +14142,8 @@
       <c r="I574" s="19">
         <v>434</v>
       </c>
-      <c r="J574" s="17">
-        <v>45</v>
+      <c r="J574" s="17" t="s">
+        <v>1324</v>
       </c>
       <c r="L574" s="19">
         <v>434</v>
@@ -14098,10 +14157,10 @@
         <v>1161</v>
       </c>
       <c r="C575" s="16" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D575" s="16" t="s">
         <v>1242</v>
+      </c>
+      <c r="D575" s="1" t="s">
+        <v>1330</v>
       </c>
       <c r="G575" s="18"/>
       <c r="H575" s="17" t="s">
@@ -14110,6 +14169,9 @@
       <c r="I575" s="19">
         <v>434</v>
       </c>
+      <c r="J575" s="17" t="s">
+        <v>1325</v>
+      </c>
       <c r="L575" s="19">
         <v>434</v>
       </c>
@@ -14119,10 +14181,10 @@
         <v>1161</v>
       </c>
       <c r="C576" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D576" s="1" t="s">
         <v>1244</v>
-      </c>
-      <c r="D576" s="1" t="s">
-        <v>1245</v>
       </c>
       <c r="H576" t="s">
         <v>70</v>
@@ -14145,10 +14207,10 @@
         <v>1161</v>
       </c>
       <c r="C577" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D577" s="1" t="s">
         <v>1246</v>
-      </c>
-      <c r="D577" s="1" t="s">
-        <v>1247</v>
       </c>
       <c r="H577" t="s">
         <v>70</v>
@@ -14171,10 +14233,10 @@
         <v>1161</v>
       </c>
       <c r="C578" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D578" s="1" t="s">
         <v>1248</v>
-      </c>
-      <c r="D578" s="1" t="s">
-        <v>1249</v>
       </c>
       <c r="H578" t="s">
         <v>70</v>
@@ -14197,10 +14259,10 @@
         <v>1161</v>
       </c>
       <c r="C579" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D579" s="1" t="s">
         <v>1250</v>
-      </c>
-      <c r="D579" s="1" t="s">
-        <v>1251</v>
       </c>
       <c r="H579" t="s">
         <v>70</v>
@@ -14223,10 +14285,10 @@
         <v>1161</v>
       </c>
       <c r="C580" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D580" s="1" t="s">
         <v>1252</v>
-      </c>
-      <c r="D580" s="1" t="s">
-        <v>1253</v>
       </c>
       <c r="H580" t="s">
         <v>70</v>
@@ -14249,10 +14311,10 @@
         <v>1161</v>
       </c>
       <c r="C581" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D581" s="1" t="s">
         <v>1254</v>
-      </c>
-      <c r="D581" s="1" t="s">
-        <v>1255</v>
       </c>
       <c r="H581" t="s">
         <v>70</v>
@@ -14275,10 +14337,10 @@
         <v>1161</v>
       </c>
       <c r="C582" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D582" s="1" t="s">
         <v>1256</v>
-      </c>
-      <c r="D582" s="1" t="s">
-        <v>1257</v>
       </c>
       <c r="H582" t="s">
         <v>70</v>
@@ -14286,14 +14348,14 @@
       <c r="I582" s="5">
         <v>434</v>
       </c>
-      <c r="J582" s="21" t="s">
-        <v>1258</v>
+      <c r="J582" s="21">
+        <v>58</v>
       </c>
       <c r="L582" s="5">
         <v>434</v>
       </c>
       <c r="M582" s="21" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="583" spans="2:13" x14ac:dyDescent="0.25">
@@ -14301,10 +14363,10 @@
         <v>1161</v>
       </c>
       <c r="C583" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D583" s="1" t="s">
         <v>1259</v>
-      </c>
-      <c r="D583" s="1" t="s">
-        <v>1260</v>
       </c>
       <c r="H583" t="s">
         <v>70</v>
@@ -14327,10 +14389,10 @@
         <v>1161</v>
       </c>
       <c r="C584" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D584" s="1" t="s">
         <v>1261</v>
-      </c>
-      <c r="D584" s="1" t="s">
-        <v>1262</v>
       </c>
       <c r="H584" t="s">
         <v>70</v>
@@ -14353,10 +14415,10 @@
         <v>1161</v>
       </c>
       <c r="C585" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D585" s="1" t="s">
         <v>1263</v>
-      </c>
-      <c r="D585" s="1" t="s">
-        <v>1264</v>
       </c>
       <c r="H585" t="s">
         <v>70</v>
@@ -14379,10 +14441,10 @@
         <v>1161</v>
       </c>
       <c r="C586" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D586" s="1" t="s">
         <v>1265</v>
-      </c>
-      <c r="D586" s="1" t="s">
-        <v>1266</v>
       </c>
       <c r="H586" t="s">
         <v>70</v>
@@ -14405,10 +14467,10 @@
         <v>1161</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="D587" s="1" t="s">
-        <v>1268</v>
+        <v>1331</v>
       </c>
       <c r="H587" t="s">
         <v>70</v>
@@ -14416,8 +14478,8 @@
       <c r="I587" s="5">
         <v>434</v>
       </c>
-      <c r="J587">
-        <v>67</v>
+      <c r="J587" t="s">
+        <v>1326</v>
       </c>
       <c r="L587" s="5">
         <v>434</v>
@@ -14431,10 +14493,10 @@
         <v>1161</v>
       </c>
       <c r="C588" s="1" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="D588" s="1" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="H588" t="s">
         <v>70</v>
@@ -14457,10 +14519,10 @@
         <v>1161</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="D589" s="1" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="H589" t="s">
         <v>70</v>
@@ -14483,10 +14545,10 @@
         <v>1161</v>
       </c>
       <c r="C590" s="1" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="H590" t="s">
         <v>70</v>
@@ -14509,10 +14571,10 @@
         <v>1161</v>
       </c>
       <c r="C591" s="1" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="D591" s="1" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="H591" t="s">
         <v>70</v>
@@ -14535,10 +14597,10 @@
         <v>1161</v>
       </c>
       <c r="C592" s="1" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="D592" s="1" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="H592" t="s">
         <v>70</v>
@@ -14561,10 +14623,10 @@
         <v>1161</v>
       </c>
       <c r="C593" s="1" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="H593" t="s">
         <v>70</v>
@@ -14587,10 +14649,10 @@
         <v>1161</v>
       </c>
       <c r="C594" s="1" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="H594" t="s">
         <v>70</v>
@@ -14613,10 +14675,10 @@
         <v>1161</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="D595" s="1" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="H595" t="s">
         <v>70</v>
@@ -14639,10 +14701,10 @@
         <v>1161</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="H596" t="s">
         <v>70</v>
@@ -14665,10 +14727,10 @@
         <v>1161</v>
       </c>
       <c r="C597" s="1" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="H597" t="s">
         <v>70</v>
@@ -14691,10 +14753,10 @@
         <v>1161</v>
       </c>
       <c r="C598" s="1" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="H598" t="s">
         <v>70</v>
@@ -14717,10 +14779,10 @@
         <v>1161</v>
       </c>
       <c r="C599" s="1" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="D599" s="1" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="H599" t="s">
         <v>70</v>
@@ -14743,10 +14805,10 @@
         <v>1161</v>
       </c>
       <c r="C600" s="1" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="H600" t="s">
         <v>70</v>
@@ -14754,8 +14816,8 @@
       <c r="I600" s="5">
         <v>434</v>
       </c>
-      <c r="J600">
-        <v>98</v>
+      <c r="J600" t="s">
+        <v>1327</v>
       </c>
       <c r="L600" s="5">
         <v>434</v>
@@ -14769,10 +14831,10 @@
         <v>1161</v>
       </c>
       <c r="C601" s="1" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="H601" t="s">
         <v>70</v>
@@ -14780,8 +14842,8 @@
       <c r="I601" s="5">
         <v>434</v>
       </c>
-      <c r="J601">
-        <v>99</v>
+      <c r="J601" t="s">
+        <v>1328</v>
       </c>
       <c r="L601" s="5">
         <v>434</v>
@@ -14790,252 +14852,312 @@
         <v>99</v>
       </c>
     </row>
-    <row r="602" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B602" s="3"/>
-      <c r="C602" s="3"/>
-      <c r="D602" s="3"/>
-      <c r="G602" s="14"/>
+    <row r="602" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B602" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D602" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="H602" t="s">
+        <v>70</v>
+      </c>
+      <c r="I602" s="5">
+        <v>434</v>
+      </c>
+      <c r="J602">
+        <v>66</v>
+      </c>
     </row>
     <row r="603" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B603" s="1" t="s">
-        <v>1297</v>
+        <v>1161</v>
       </c>
       <c r="C603" s="1" t="s">
-        <v>1152</v>
+        <v>1334</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>1298</v>
+        <v>1335</v>
+      </c>
+      <c r="H603" t="s">
+        <v>70</v>
+      </c>
+      <c r="I603" s="5">
+        <v>434</v>
+      </c>
+      <c r="J603">
+        <v>83</v>
       </c>
     </row>
     <row r="604" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B604" s="1" t="s">
-        <v>1297</v>
+        <v>1161</v>
       </c>
       <c r="C604" s="1" t="s">
-        <v>1154</v>
+        <v>1336</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="605" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B605" s="1" t="s">
-        <v>1297</v>
-      </c>
-      <c r="C605" s="1" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D605" s="1" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="606" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B606" s="3"/>
-      <c r="C606" s="3"/>
-      <c r="D606" s="3"/>
-      <c r="G606" s="14"/>
+        <v>1337</v>
+      </c>
+      <c r="H604" t="s">
+        <v>70</v>
+      </c>
+      <c r="I604" s="5">
+        <v>434</v>
+      </c>
+      <c r="J604">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="605" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B605" s="3"/>
+      <c r="C605" s="3"/>
+      <c r="D605" s="3"/>
+      <c r="G605" s="14"/>
+    </row>
+    <row r="606" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B606" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D606" s="1" t="s">
+        <v>1296</v>
+      </c>
     </row>
     <row r="607" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B607" s="1" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>1302</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="608" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B608" s="1" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="609" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B609" s="1" t="s">
-        <v>1301</v>
-      </c>
-      <c r="C609" s="1" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D609" s="1" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="610" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B610" s="3"/>
-      <c r="C610" s="3"/>
-      <c r="D610" s="3"/>
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="609" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B609" s="3"/>
+      <c r="C609" s="3"/>
+      <c r="D609" s="3"/>
+      <c r="G609" s="14"/>
+    </row>
+    <row r="610" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B610" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D610" s="1" t="s">
+        <v>1300</v>
+      </c>
     </row>
     <row r="611" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B611" s="1" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="C611" s="1" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="D611" s="1" t="s">
-        <v>1306</v>
-      </c>
-      <c r="H611" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I611" s="22">
-        <v>564</v>
-      </c>
-      <c r="J611" s="12">
-        <v>3</v>
-      </c>
-      <c r="L611" s="22">
-        <v>564</v>
-      </c>
-      <c r="M611" s="12">
-        <v>3</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="612" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B612" s="1" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="C612" s="1" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D612" s="1" t="s">
-        <v>1307</v>
-      </c>
-      <c r="H612" s="7" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="613" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B613" s="3"/>
+      <c r="C613" s="3"/>
+      <c r="D613" s="3"/>
+    </row>
+    <row r="614" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B614" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D614" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="H614" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I612" s="5">
+      <c r="I614" s="22">
         <v>564</v>
       </c>
-      <c r="J612">
-        <v>2</v>
-      </c>
-      <c r="L612" s="5">
+      <c r="J614" s="12">
+        <v>3</v>
+      </c>
+      <c r="L614" s="22">
         <v>564</v>
       </c>
-      <c r="M612">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="613" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B613" s="1" t="s">
-        <v>1305</v>
-      </c>
-      <c r="C613" s="1" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D613" s="1" t="s">
-        <v>1308</v>
-      </c>
-      <c r="H613" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I613" s="22">
-        <v>564</v>
-      </c>
-      <c r="J613" s="23">
-        <v>1</v>
-      </c>
-      <c r="L613" s="22">
-        <v>564</v>
-      </c>
-      <c r="M613" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="614" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B614" s="3"/>
-      <c r="C614" s="3"/>
-      <c r="D614" s="3"/>
-      <c r="G614" s="14"/>
+      <c r="M614" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="615" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B615" s="1" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="C615" s="1" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>1310</v>
+        <v>1305</v>
+      </c>
+      <c r="H615" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I615" s="5">
+        <v>564</v>
+      </c>
+      <c r="J615">
+        <v>2</v>
+      </c>
+      <c r="L615" s="5">
+        <v>564</v>
+      </c>
+      <c r="M615">
+        <v>2</v>
       </c>
     </row>
     <row r="616" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B616" s="1" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="617" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B617" s="1" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C617" s="1" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D617" s="1" t="s">
-        <v>1312</v>
-      </c>
+        <v>1306</v>
+      </c>
+      <c r="H616" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I616" s="22">
+        <v>564</v>
+      </c>
+      <c r="J616" s="23">
+        <v>1</v>
+      </c>
+      <c r="L616" s="22">
+        <v>564</v>
+      </c>
+      <c r="M616" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="617" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B617" s="3"/>
+      <c r="C617" s="3"/>
+      <c r="D617" s="3"/>
+      <c r="G617" s="14"/>
     </row>
     <row r="618" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B618" s="1" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>1313</v>
+        <v>1152</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="619" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B619" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D619" s="1" t="s">
         <v>1309</v>
-      </c>
-      <c r="C619" s="1" t="s">
-        <v>1315</v>
-      </c>
-      <c r="D619" s="1" t="s">
-        <v>1316</v>
       </c>
     </row>
     <row r="620" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B620" s="1" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C620" s="1" t="s">
-        <v>1317</v>
+        <v>1156</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>1318</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="621" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B621" s="1" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C621" s="1" t="s">
-        <v>1319</v>
+        <v>1311</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="622" spans="2:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G622" s="14"/>
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="622" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B622" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D622" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="623" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B623" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D623" s="1" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="624" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B624" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D624" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="625" spans="7:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G625" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>